<commit_message>
Update 5-) Turkiye'nin tekstilde ihracat ve ithalat.xlsx
</commit_message>
<xml_diff>
--- a/5-) Turkiye'nin tekstilde ihracat ve ithalat.xlsx
+++ b/5-) Turkiye'nin tekstilde ihracat ve ithalat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fintegral365-my.sharepoint.com/personal/oguz_oztekin_fintegral_com_tr/Documents/Masaüstü/Dis-Ticaret-Tekstil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_0BC37929F8998775407E687B3D4825CDEE7B1295" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{328AF4E6-A346-422B-AFA5-AF36C570D508}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_0BC37929F8998775407E687B3D4825CDEE7B1295" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E444CFB7-786B-4D4B-8307-5D93B836A02D}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15030" yWindow="885" windowWidth="12420" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2012_İhracat" sheetId="1" r:id="rId1"/>
@@ -631,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -665,12 +665,8 @@
       <c r="C2">
         <v>15.19679258036988</v>
       </c>
-      <c r="E2">
-        <f>SUM(C2:C41)</f>
-        <v>89.885546641910906</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -681,7 +677,7 @@
         <v>9.1629685800555674</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -692,7 +688,7 @@
         <v>6.0942322826738717</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -703,7 +699,7 @@
         <v>5.7669514689407491</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -714,7 +710,7 @@
         <v>5.1797936339736914</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -725,7 +721,7 @@
         <v>5.1194754774779554</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -736,7 +732,7 @@
         <v>4.1247228186226854</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -747,7 +743,7 @@
         <v>3.6805641902892838</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -758,7 +754,7 @@
         <v>3.5162238875088669</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -769,7 +765,7 @@
         <v>2.5110342954317821</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -780,7 +776,7 @@
         <v>2.0176701053706769</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -791,7 +787,7 @@
         <v>1.854346110927489</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -802,7 +798,7 @@
         <v>1.819971683148037</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -813,7 +809,7 @@
         <v>1.5844999576852861</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -5746,15 +5742,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5765,7 +5761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5775,12 +5771,8 @@
       <c r="C2">
         <v>26.835583466027501</v>
       </c>
-      <c r="E2">
-        <f>SUM(C2:C41)</f>
-        <v>96.284581939366788</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5791,7 +5783,7 @@
         <v>6.4228976427677038</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5802,7 +5794,7 @@
         <v>6.1361297260804371</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -5813,7 +5805,7 @@
         <v>6.0633135978069754</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -5824,7 +5816,7 @@
         <v>5.9233248143769428</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5835,7 +5827,7 @@
         <v>5.4753533517704627</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -5846,7 +5838,7 @@
         <v>4.9138036434395431</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -5857,7 +5849,7 @@
         <v>4.5341825103733981</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -5868,7 +5860,7 @@
         <v>2.868003559483367</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -5879,7 +5871,7 @@
         <v>2.3461658252367461</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -5890,7 +5882,7 @@
         <v>2.130081434019206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -5901,7 +5893,7 @@
         <v>1.9820544220072349</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -5912,7 +5904,7 @@
         <v>1.865277028560707</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -5923,7 +5915,7 @@
         <v>1.7245248782395719</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -6680,10 +6672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6694,7 +6686,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6705,7 +6697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6715,12 +6707,8 @@
       <c r="C2">
         <v>15.002614100322459</v>
       </c>
-      <c r="E2">
-        <f>SUM(C2:C41)</f>
-        <v>89.136085940828295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6731,7 +6719,7 @@
         <v>8.2675673213549103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6742,7 +6730,7 @@
         <v>5.8996286773714202</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6753,7 +6741,7 @@
         <v>5.2069751185209254</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -6764,7 +6752,7 @@
         <v>5.0848878771341566</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6775,7 +6763,7 @@
         <v>5.0740019930402394</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6786,7 +6774,7 @@
         <v>4.5412370657745127</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -6797,7 +6785,7 @@
         <v>3.64196097145257</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6808,7 +6796,7 @@
         <v>3.575821569783765</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -6819,7 +6807,7 @@
         <v>2.397831324608815</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -6830,7 +6818,7 @@
         <v>2.2294983318147938</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6841,7 +6829,7 @@
         <v>1.976356185916645</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -6852,7 +6840,7 @@
         <v>1.9674112747898891</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -6863,7 +6851,7 @@
         <v>1.829405794485895</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>